<commit_message>
Added single doctype elaconfiguration - initial use is to hold the list of suppported templates A/S/M.  Logic to identify template based on question config and sequence and validate. Updates to filenames to reflect template string names.
</commit_message>
<xml_diff>
--- a/ela/templates/ELA_FORM_TMPL_A1S1.xlsx
+++ b/ela/templates/ELA_FORM_TMPL_A1S1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -305,27 +305,9 @@
     <t xml:space="preserve">assessments</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The following {{ assessment_count }} assessment(s) are included in this form
-{{ question_types[0] }}: {{ ela_asssessment_ids[0]  }}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">{{ question_types[1] }}: {{ ela_asssessment_ids[1]  }}</t>
-    </r>
+    <t xml:space="preserve">The following {{ assessment_count }} assessment(s) are included in this form
+{{ question_types[0] }}: {{ assessment_ids[0]  }}
+{{ question_types[1] }}: {{ assessment_ids[1]  }}</t>
   </si>
   <si>
     <t xml:space="preserve">num_assessments</t>
@@ -388,10 +370,10 @@
     <t xml:space="preserve">{{ question_prompts[0] }}</t>
   </si>
   <si>
-    <t xml:space="preserve">ela_asssessment_id_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“{{ ela_asssessment_ids[0] }}”</t>
+    <t xml:space="preserve">assessment_id_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“{{ assessment_ids[0] }}”</t>
   </si>
   <si>
     <t xml:space="preserve">question_1_type</t>
@@ -427,10 +409,10 @@
     <t xml:space="preserve">{{ question_prompts[1] }}</t>
   </si>
   <si>
-    <t xml:space="preserve">ela_asssessment_id_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“{{ ela_asssessment_ids[1] }}”</t>
+    <t xml:space="preserve">assessment_id_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“{{ assessment_ids[1] }}”</t>
   </si>
   <si>
     <t xml:space="preserve">question_2_type</t>
@@ -548,7 +530,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -578,12 +560,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -664,11 +640,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,15 +667,15 @@
   </sheetPr>
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -1114,7 +1090,7 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -1122,7 +1098,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.63"/>
@@ -1351,7 +1327,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.13"/>
@@ -1428,7 +1404,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.95703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">

</xml_diff>